<commit_message>
Play mechanics and db mechanics functional
</commit_message>
<xml_diff>
--- a/DB/ARI_Bloomquist_Willie.xlsx
+++ b/DB/ARI_Bloomquist_Willie.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>lastname</t>
   </si>
@@ -35,7 +35,10 @@
     <t>vsrh</t>
   </si>
   <si>
-    <t>play</t>
+    <t>play_vslh</t>
+  </si>
+  <si>
+    <t>play_vsrh</t>
   </si>
   <si>
     <t>bloomquist</t>
@@ -128,6 +131,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -209,10 +213,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -242,19 +246,22 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>10</v>
@@ -263,7 +270,10 @@
         <v>10</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -274,7 +284,10 @@
         <v>67</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -285,7 +298,10 @@
         <v>82</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -296,7 +312,10 @@
         <v>97</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,7 +326,10 @@
         <v>127</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -318,7 +340,10 @@
         <v>129</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,7 +354,10 @@
         <v>164</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,7 +368,10 @@
         <v>187</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,7 +382,10 @@
         <v>199</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -362,7 +396,10 @@
         <v>201</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,7 +410,10 @@
         <v>263</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,7 +424,10 @@
         <v>325</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,7 +438,10 @@
         <v>371</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -406,7 +452,10 @@
         <v>386</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,7 +466,10 @@
         <v>393</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -428,7 +480,10 @@
         <v>409</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -439,7 +494,10 @@
         <v>412</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,7 +508,10 @@
         <v>413</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,7 +522,10 @@
         <v>415</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,7 +536,10 @@
         <v>471</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -483,7 +550,10 @@
         <v>490</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -494,7 +564,10 @@
         <v>499</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>